<commit_message>
updating with a couple things
</commit_message>
<xml_diff>
--- a/py_outputs/snip.xlsx
+++ b/py_outputs/snip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/big_team_who/py_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFF4CFC4-3B4F-5144-BADD-8E7C9762A7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2854F8-6FBA-DF44-BF38-C9C4468EBE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="700" windowWidth="26740" windowHeight="16260" xr2:uid="{CD2464BA-E537-B04A-9EF8-BAC31AE88FD0}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,16 +453,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.3984844972471704</v>
+        <v>2.3796008642440598</v>
       </c>
       <c r="C2">
-        <v>7.1846479513521597</v>
+        <v>3.6918003194439302</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2.0779999999999998</v>
+        <v>1.5780000000000001</v>
       </c>
       <c r="F2">
         <v>173.93199999999999</v>
@@ -473,16 +473,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.7298434289762601</v>
+        <v>1.55897105099264</v>
       </c>
       <c r="C3">
-        <v>1.33667236834595</v>
+        <v>1.1699381174883601</v>
       </c>
       <c r="D3">
-        <v>0.155</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1.278</v>
+        <v>1.2589999999999999</v>
       </c>
       <c r="F3">
         <v>30.405000000000001</v>
@@ -493,16 +493,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6.0929441233140604</v>
+        <v>3.5859652166517799</v>
       </c>
       <c r="C4">
-        <v>4.3151334953509002</v>
+        <v>3.6116202332824399</v>
       </c>
       <c r="D4">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>3.3410000000000002</v>
+        <v>1.389</v>
       </c>
       <c r="F4">
         <v>11.342000000000001</v>
@@ -513,16 +513,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.2047848605577598</v>
+        <v>1.9287925424064001</v>
       </c>
       <c r="C5">
-        <v>2.1441319264666698</v>
+        <v>1.7164829247606299</v>
       </c>
       <c r="D5">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1.605</v>
+        <v>1.5229999999999999</v>
       </c>
       <c r="F5">
         <v>30.405000000000001</v>
@@ -533,19 +533,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.5242472490150698</v>
+        <v>2.02502948617445</v>
       </c>
       <c r="C6">
-        <v>2.04489898808432</v>
+        <v>1.6086746094601101</v>
       </c>
       <c r="D6">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1.742</v>
+        <v>1.5069999999999999</v>
       </c>
       <c r="F6">
-        <v>12.624000000000001</v>
+        <v>14.856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>